<commit_message>
started working on scripts for baseline to novote intervention. none of this is tested, and it is not complete
</commit_message>
<xml_diff>
--- a/GCP/txt_ctr_table.xlsx
+++ b/GCP/txt_ctr_table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amywinecoff/Documents/CITP/Research/Github/citp-sm-politics/GCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858745E8-8A69-9D4C-B9CA-72D736B39291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F1CB5-F2E9-554E-BE92-06D16E300FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{E5191F5B-E78B-0142-AA5E-9D8552D7B311}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>treatment subreddit</t>
   </si>
@@ -175,14 +175,18 @@
   <si>
     <t>\democrats</t>
   </si>
+  <si>
+    <t>\iran</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -245,13 +249,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -567,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0478B043-AFA5-1544-BDBE-C02DC27C5DA2}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,9 +587,9 @@
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,10 +606,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -617,7 +626,7 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>15377027</v>
       </c>
       <c r="F2" s="4">
@@ -629,13 +638,7 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>106334</v>
       </c>
       <c r="F3" s="4">
@@ -647,89 +650,66 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1277109</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1236675</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="E5" s="5">
         <v>700000</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="4">
         <v>1811176</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E5" s="4"/>
-      <c r="G5"/>
-    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4">
-        <v>154983</v>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5">
+        <v>74685</v>
       </c>
       <c r="F6" s="4">
-        <v>131941</v>
-      </c>
-      <c r="G6"/>
+        <v>77923</v>
+      </c>
+      <c r="G6">
+        <v>0.99199999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5">
-        <v>32898</v>
-      </c>
-      <c r="F7" s="4">
-        <v>14449</v>
+        <v>130847</v>
+      </c>
+      <c r="F7" s="7">
+        <v>270821</v>
       </c>
       <c r="G7">
-        <v>0.998</v>
+        <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4">
-        <v>19877</v>
-      </c>
-      <c r="F8" s="4">
-        <v>18069</v>
-      </c>
-      <c r="G8">
-        <v>0.995</v>
-      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7"/>
+      <c r="G8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>28</v>
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -737,143 +717,120 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="4">
-        <v>22821</v>
+      <c r="E9" s="5">
+        <v>154983</v>
       </c>
       <c r="F9" s="4">
-        <v>19745</v>
-      </c>
-      <c r="G9">
+        <v>131941</v>
+      </c>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="9">
+        <v>32898</v>
+      </c>
+      <c r="F10" s="4">
+        <v>14449</v>
+      </c>
+      <c r="G10">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5">
+        <v>19877</v>
+      </c>
+      <c r="F11" s="4">
+        <v>18069</v>
+      </c>
+      <c r="G11">
         <v>0.995</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="4"/>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4">
-        <v>9698</v>
-      </c>
-      <c r="F11" s="4">
-        <v>970218</v>
-      </c>
-      <c r="G11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="5">
+        <v>22821</v>
+      </c>
+      <c r="F12" s="4">
+        <v>19745</v>
+      </c>
+      <c r="G12">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="5">
+        <f>SUM(E10:E12)/E9</f>
+        <v>0.48776962634611537</v>
+      </c>
+      <c r="F13" s="4">
+        <f>SUM(F10:F12)/F9</f>
+        <v>0.39610886684199759</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="5">
+        <v>9698</v>
+      </c>
+      <c r="F14" s="4">
+        <v>970218</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="E15" s="5">
         <v>8477</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F15" s="4">
         <v>68695</v>
       </c>
-      <c r="G12">
+      <c r="G15">
         <v>0.97299999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="4">
-        <v>65374</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1094388</v>
-      </c>
-      <c r="G13">
-        <v>0.96299999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="4"/>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="4">
-        <v>14032370</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2070909</v>
-      </c>
-      <c r="G15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E16" s="5">
-        <v>560327</v>
+        <v>65374</v>
       </c>
       <c r="F16" s="4">
-        <v>477218</v>
+        <v>1094388</v>
       </c>
       <c r="G16">
-        <v>0.97699999999999998</v>
+        <v>0.96299999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="5">
-        <v>476074</v>
-      </c>
-      <c r="F17" s="4">
-        <v>278502</v>
-      </c>
-      <c r="G17">
-        <v>0.97399999999999998</v>
-      </c>
+      <c r="E17" s="5"/>
+      <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>32</v>
+      <c r="A18" t="s">
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -881,102 +838,82 @@
       <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="4">
-        <v>782363</v>
+      <c r="E18" s="5">
+        <v>14032370</v>
       </c>
       <c r="F18" s="4">
-        <v>253573</v>
-      </c>
-      <c r="G18">
-        <v>0.95399999999999996</v>
-      </c>
+        <v>2070909</v>
+      </c>
+      <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1148535</v>
+        <v>31</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="E19" s="9">
+        <v>476074</v>
       </c>
       <c r="F19" s="4">
-        <v>756534</v>
+        <v>278502</v>
       </c>
       <c r="G19">
-        <v>0.99299999999999999</v>
+        <v>0.97399999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="E20" s="5">
+        <v>782363</v>
+      </c>
+      <c r="F20" s="4">
+        <v>253573</v>
+      </c>
+      <c r="G20">
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="E21" s="5">
+        <v>1148535</v>
+      </c>
+      <c r="F21" s="4">
+        <v>756534</v>
+      </c>
+      <c r="G21">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="C22" s="2"/>
+      <c r="E22" s="5">
         <v>361532</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F22" s="4">
         <v>13974</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="4">
-        <v>595865</v>
-      </c>
-      <c r="F22" s="4">
-        <v>4956857</v>
-      </c>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="4">
-        <v>111141</v>
-      </c>
-      <c r="F23" s="4">
-        <v>290487</v>
-      </c>
-      <c r="G23">
-        <v>0.97399999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -984,53 +921,53 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="4">
-        <v>140426</v>
+      <c r="E24" s="5">
+        <v>595865</v>
       </c>
       <c r="F24" s="4">
-        <v>114329</v>
-      </c>
-      <c r="G24">
-        <v>0.95799999999999996</v>
-      </c>
+        <v>4956857</v>
+      </c>
+      <c r="G24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="4">
-        <v>41681</v>
+        <v>35</v>
+      </c>
+      <c r="E25" s="5">
+        <v>140426</v>
       </c>
       <c r="F25" s="4">
-        <v>44485</v>
+        <v>114329</v>
       </c>
       <c r="G25">
-        <v>0.95499999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="5">
+        <v>41681</v>
+      </c>
+      <c r="F26" s="4">
+        <v>44485</v>
+      </c>
+      <c r="G26">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="E27" s="9">
         <v>35964</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F27" s="4">
         <v>177714</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0.94299999999999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added code to create no vote intervention tables. currently vegan is not in it because there is no intervention data. started intervention table for upvote to novotes
</commit_message>
<xml_diff>
--- a/GCP/txt_ctr_table.xlsx
+++ b/GCP/txt_ctr_table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amywinecoff/Documents/CITP/Research/Github/citp-sm-politics/GCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F1CB5-F2E9-554E-BE92-06D16E300FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7658159-8398-4840-AF75-A4872B0E46DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{E5191F5B-E78B-0142-AA5E-9D8552D7B311}"/>
+    <workbookView xWindow="-34960" yWindow="6080" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{E5191F5B-E78B-0142-AA5E-9D8552D7B311}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="baseline_upvote" sheetId="1" r:id="rId1"/>
+    <sheet name="baseline_novote" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>treatment subreddit</t>
   </si>
@@ -177,6 +178,35 @@
   </si>
   <si>
     <t>\iran</t>
+  </si>
+  <si>
+    <t>\unpopularopinion</t>
+  </si>
+  <si>
+    <t>02-21-2018 to 04-01-2018</t>
+  </si>
+  <si>
+    <t>01-01-2010 to 02-20-2018</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no votes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+  </si>
+  <si>
+    <t>no votes dates</t>
   </si>
 </sst>
 </file>
@@ -578,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0478B043-AFA5-1544-BDBE-C02DC27C5DA2}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,4 +1004,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371DAE90-057D-DB47-917C-986F5749827F}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="5">
+        <v>612169</v>
+      </c>
+      <c r="F2" s="4">
+        <v>151280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="5">
+        <v>1519118</v>
+      </c>
+      <c r="F3" s="4">
+        <v>210184</v>
+      </c>
+      <c r="G3">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code successfully runs for the upvote to novote tables. added a bit more documentation
</commit_message>
<xml_diff>
--- a/GCP/txt_ctr_table.xlsx
+++ b/GCP/txt_ctr_table.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amywinecoff/Documents/CITP/Research/Github/citp-sm-politics/GCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7658159-8398-4840-AF75-A4872B0E46DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EB11C-A058-AA43-9835-5DED50ADAA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34960" yWindow="6080" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{E5191F5B-E78B-0142-AA5E-9D8552D7B311}"/>
+    <workbookView xWindow="-34960" yWindow="6080" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{E5191F5B-E78B-0142-AA5E-9D8552D7B311}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline_upvote" sheetId="1" r:id="rId1"/>
     <sheet name="baseline_novote" sheetId="2" r:id="rId2"/>
+    <sheet name="upvote_novote" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>treatment subreddit</t>
   </si>
@@ -207,6 +208,47 @@
   </si>
   <si>
     <t>no votes dates</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">novote </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+  </si>
+  <si>
+    <t>2013-11-01 to 2014-06-30</t>
+  </si>
+  <si>
+    <t>no vote dates</t>
+  </si>
+  <si>
+    <t>2014-07-01 to 2018-01-01</t>
+  </si>
+  <si>
+    <t>\GenderCritical</t>
+  </si>
+  <si>
+    <t>2014-07-01 to 2018-04-01</t>
+  </si>
+  <si>
+    <t>2013-10-03 to 2014-06-30</t>
+  </si>
+  <si>
+    <t>2014-01-30 to 2014-12-29</t>
+  </si>
+  <si>
+    <t>2014-12-30 to 2018-04-01</t>
   </si>
 </sst>
 </file>
@@ -279,11 +321,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -291,6 +334,9 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -617,8 +663,8 @@
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -636,10 +682,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -656,10 +702,10 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>15377027</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>3478327</v>
       </c>
       <c r="G2"/>
@@ -668,10 +714,10 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>106334</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>1631444</v>
       </c>
       <c r="G3">
@@ -682,10 +728,10 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>1277109</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>1236675</v>
       </c>
       <c r="G4"/>
@@ -694,10 +740,10 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>700000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>1811176</v>
       </c>
       <c r="G5">
@@ -708,10 +754,10 @@
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>74685</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>77923</v>
       </c>
       <c r="G6">
@@ -722,10 +768,10 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>130847</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>270821</v>
       </c>
       <c r="G7">
@@ -733,8 +779,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -747,10 +793,10 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>154983</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>131941</v>
       </c>
       <c r="G9"/>
@@ -759,10 +805,10 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="10">
         <v>32898</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>14449</v>
       </c>
       <c r="G10">
@@ -773,10 +819,10 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>19877</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>18069</v>
       </c>
       <c r="G11">
@@ -787,10 +833,10 @@
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>22821</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <v>19745</v>
       </c>
       <c r="G12">
@@ -798,11 +844,11 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="5">
+      <c r="E13" s="6">
         <f>SUM(E10:E12)/E9</f>
         <v>0.48776962634611537</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <f>SUM(F10:F12)/F9</f>
         <v>0.39610886684199759</v>
       </c>
@@ -818,10 +864,10 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>9698</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <v>970218</v>
       </c>
       <c r="G14"/>
@@ -830,10 +876,10 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>8477</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="5">
         <v>68695</v>
       </c>
       <c r="G15">
@@ -844,10 +890,10 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>65374</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="5">
         <v>1094388</v>
       </c>
       <c r="G16">
@@ -855,7 +901,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E17" s="5"/>
+      <c r="E17" s="6"/>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -868,10 +914,10 @@
       <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>14032370</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="5">
         <v>2070909</v>
       </c>
       <c r="G18"/>
@@ -881,10 +927,10 @@
         <v>31</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="E19" s="9">
+      <c r="E19" s="10">
         <v>476074</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="5">
         <v>278502</v>
       </c>
       <c r="G19">
@@ -896,10 +942,10 @@
         <v>32</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="5">
+      <c r="E20" s="6">
         <v>782363</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="5">
         <v>253573</v>
       </c>
       <c r="G20">
@@ -911,10 +957,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="E21" s="5">
+      <c r="E21" s="6">
         <v>1148535</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="5">
         <v>756534</v>
       </c>
       <c r="G21">
@@ -926,10 +972,10 @@
         <v>33</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="E22" s="5">
+      <c r="E22" s="6">
         <v>361532</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="5">
         <v>13974</v>
       </c>
       <c r="G22">
@@ -938,7 +984,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C23" s="2"/>
-      <c r="E23" s="5"/>
+      <c r="E23" s="6"/>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -951,10 +997,10 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>595865</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="5">
         <v>4956857</v>
       </c>
       <c r="G24"/>
@@ -963,10 +1009,10 @@
       <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>140426</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="5">
         <v>114329</v>
       </c>
       <c r="G25">
@@ -977,10 +1023,10 @@
       <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="6">
         <v>41681</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="5">
         <v>44485</v>
       </c>
       <c r="G26">
@@ -991,10 +1037,10 @@
       <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="10">
         <v>35964</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="5">
         <v>177714</v>
       </c>
       <c r="G27">
@@ -1010,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371DAE90-057D-DB47-917C-986F5749827F}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1037,10 +1083,10 @@
       <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1057,10 +1103,10 @@
       <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>612169</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>151280</v>
       </c>
     </row>
@@ -1070,14 +1116,250 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>1519118</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>210184</v>
       </c>
       <c r="G3">
         <v>0.97899999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73375ACA-1C1F-8C46-B11D-3A6382E311AA}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="6">
+        <v>131941</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1535763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="6">
+        <v>24238</v>
+      </c>
+      <c r="F3" s="5">
+        <v>131108</v>
+      </c>
+      <c r="G3">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4">
+        <v>19745</v>
+      </c>
+      <c r="F4" s="4">
+        <v>96124</v>
+      </c>
+      <c r="G4">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4">
+        <v>14449</v>
+      </c>
+      <c r="F5" s="4">
+        <v>205248</v>
+      </c>
+      <c r="G5">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="4">
+        <v>7857</v>
+      </c>
+      <c r="F7" s="4">
+        <v>429107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="4">
+        <v>15035</v>
+      </c>
+      <c r="F8" s="4">
+        <v>123372</v>
+      </c>
+      <c r="G8">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2070909</v>
+      </c>
+      <c r="F10" s="4">
+        <v>50203736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4">
+        <v>278502</v>
+      </c>
+      <c r="F11" s="4">
+        <v>931707</v>
+      </c>
+      <c r="G11">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4">
+        <v>40575</v>
+      </c>
+      <c r="F12" s="4">
+        <v>295572</v>
+      </c>
+      <c r="G12">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4">
+        <v>756534</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3420420</v>
+      </c>
+      <c r="G13">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4">
+        <v>253573</v>
+      </c>
+      <c r="F14" s="4">
+        <v>791679</v>
+      </c>
+      <c r="G14">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4">
+        <v>477218</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1474394</v>
+      </c>
+      <c r="G15">
+        <v>0.97299999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4">
+        <v>27013</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1645018</v>
+      </c>
+      <c r="G16">
+        <v>0.96799999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>